<commit_message>
Updated user roles matrix with 1-5
</commit_message>
<xml_diff>
--- a/Documentation/User roles.xlsx
+++ b/Documentation/User roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guga/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/promieyutasane/Desktop/strataly/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A67F8A-9F4F-8749-9845-3A0B59AD5A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF626A-8BEC-404B-90DD-7CAA83CD0BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="24600" windowHeight="15000" xr2:uid="{17FE36FC-B10E-C840-9DD8-D0DF35E5259F}"/>
+    <workbookView xWindow="-28760" yWindow="-480" windowWidth="24600" windowHeight="15000" xr2:uid="{17FE36FC-B10E-C840-9DD8-D0DF35E5259F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Strataly Admin</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>Unauthorized</t>
+  </si>
+  <si>
+    <t>Role (Int)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +97,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
@@ -115,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -207,11 +218,13 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -219,6 +232,64 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -227,7 +298,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -240,7 +311,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -252,74 +323,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -328,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,31 +386,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,153 +738,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F39204-C210-4744-9FFF-E1EEF825A193}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
+    <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+    <row r="2" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="18">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="18">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="18">
+        <v>5</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated User roles and CRUD table
Updated User roles and CRUD table to fix privileges relating to User table.
</commit_message>
<xml_diff>
--- a/Documentation/User roles.xlsx
+++ b/Documentation/User roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/promieyutasane/Desktop/strataly/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guga/dev/GitHub/strataly/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AF626A-8BEC-404B-90DD-7CAA83CD0BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1448B1-066C-214F-B7C7-B6A432B44ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28760" yWindow="-480" windowWidth="24600" windowHeight="15000" xr2:uid="{17FE36FC-B10E-C840-9DD8-D0DF35E5259F}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" xr2:uid="{17FE36FC-B10E-C840-9DD8-D0DF35E5259F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>Strataly Admin</t>
   </si>
@@ -72,9 +72,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>* limited to their own unit</t>
-  </si>
-  <si>
     <t>ROLE \ RIGHTS</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>Role (Int)</t>
+  </si>
+  <si>
+    <t>RU*</t>
+  </si>
+  <si>
+    <t>* limited to registries associated with their own users</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -297,7 +300,69 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -310,7 +375,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -318,51 +385,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -407,23 +429,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,14 +763,16 @@
   <dimension ref="B1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="14" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -759,11 +783,11 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>14</v>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>4</v>
@@ -779,10 +803,10 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="18">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -799,10 +823,10 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="18">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -819,17 +843,17 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="18">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -839,17 +863,17 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="18">
+      <c r="B6" s="15">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -859,17 +883,17 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="18">
+      <c r="B7" s="15">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -879,9 +903,9 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="15" t="s">
-        <v>15</v>
+      <c r="B8" s="16"/>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>12</v>
@@ -898,11 +922,11 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>